<commit_message>
added the functionality for authors used to accuracy and min books to accuracy
</commit_message>
<xml_diff>
--- a/singleParam.xlsx
+++ b/singleParam.xlsx
@@ -1289,16 +1289,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>161926</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1586,7 +1586,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+      <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added single and adding features on accuracy
</commit_message>
<xml_diff>
--- a/singleParam.xlsx
+++ b/singleParam.xlsx
@@ -26,90 +26,27 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
-    <t>and</t>
-  </si>
-  <si>
-    <t>if</t>
-  </si>
-  <si>
     <t>averageParagraphLength</t>
   </si>
   <si>
-    <t>this</t>
-  </si>
-  <si>
-    <t>but</t>
-  </si>
-  <si>
     <t>bigraph-lc</t>
   </si>
   <si>
     <t>bigraph-we</t>
   </si>
   <si>
-    <t>might</t>
-  </si>
-  <si>
-    <t>,</t>
-  </si>
-  <si>
     <t>numberOfWords</t>
   </si>
   <si>
-    <t>more</t>
-  </si>
-  <si>
-    <t>--</t>
-  </si>
-  <si>
-    <t>!</t>
-  </si>
-  <si>
-    <t>very</t>
-  </si>
-  <si>
-    <t>;</t>
-  </si>
-  <si>
     <t>apostrophesPerWord</t>
   </si>
   <si>
-    <t>must</t>
-  </si>
-  <si>
-    <t>since</t>
-  </si>
-  <si>
     <t>bigraph-me</t>
   </si>
   <si>
-    <t xml:space="preserve">" </t>
-  </si>
-  <si>
     <t>whitespaceFraction</t>
   </si>
   <si>
-    <t>however</t>
-  </si>
-  <si>
-    <t>awps</t>
-  </si>
-  <si>
-    <t>awl</t>
-  </si>
-  <si>
-    <t>:</t>
-  </si>
-  <si>
-    <t>because</t>
-  </si>
-  <si>
-    <t>that</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>digitFraction</t>
   </si>
   <si>
@@ -117,6 +54,69 @@
   </si>
   <si>
     <t>uppercaseFraction</t>
+  </si>
+  <si>
+    <t>WPT-because</t>
+  </si>
+  <si>
+    <t>WPT-since</t>
+  </si>
+  <si>
+    <t>WPT-colon</t>
+  </si>
+  <si>
+    <t>WPT-must</t>
+  </si>
+  <si>
+    <t>WPT-this</t>
+  </si>
+  <si>
+    <t>averageWordsPerSentence</t>
+  </si>
+  <si>
+    <t>averageWordLength</t>
+  </si>
+  <si>
+    <t>WPT-doubleHyphen</t>
+  </si>
+  <si>
+    <t>WPT-exclamationMark</t>
+  </si>
+  <si>
+    <t>WPT-more</t>
+  </si>
+  <si>
+    <t>WPT-comma</t>
+  </si>
+  <si>
+    <t>WPT-however</t>
+  </si>
+  <si>
+    <t>WPT-and</t>
+  </si>
+  <si>
+    <t>WPT-very</t>
+  </si>
+  <si>
+    <t>WPT-but</t>
+  </si>
+  <si>
+    <t>WPT-if</t>
+  </si>
+  <si>
+    <t>WPT-quote</t>
+  </si>
+  <si>
+    <t>WPT-hyphen</t>
+  </si>
+  <si>
+    <t>WPT-that</t>
+  </si>
+  <si>
+    <t>WPT-might</t>
+  </si>
+  <si>
+    <t>WPT-semicolon</t>
   </si>
 </sst>
 </file>
@@ -206,8 +206,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Single Parameter Classifier</a:t>
+              <a:t>Impace</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of a Single Feature on Accuracy</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -267,94 +272,94 @@
               <c:strCache>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>and</c:v>
+                  <c:v>WPT-semicolon</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>:</c:v>
+                  <c:v>WPT-and</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>that</c:v>
+                  <c:v>WPT-that</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>;</c:v>
+                  <c:v>WPT-colon</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>but</c:v>
+                  <c:v>WPT-but</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>WPT-this</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>WPT-very</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>WPT-if</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>WPT-exclamationMark</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>digitFraction</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>this</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>very</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>--</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>if</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>more</c:v>
+                  <c:v>WPT-doubleHyphen</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>,</c:v>
+                  <c:v>WPT-more</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-</c:v>
+                  <c:v>WPT-however</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>!</c:v>
+                  <c:v>WPT-comma</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>numberOfWords</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>must</c:v>
+                  <c:v>WPT-hyphen</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>however</c:v>
+                  <c:v>WPT-must</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>averageWordsPerSentence</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>whitespaceFraction</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>awl</c:v>
-                </c:pt>
                 <c:pt idx="19">
-                  <c:v>because</c:v>
+                  <c:v>WPT-because</c:v>
                 </c:pt>
                 <c:pt idx="20">
+                  <c:v>WPT-might</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>uppercaseFraction</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>bigraph-lc</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
+                  <c:v>averageParagraphLength</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>bigraph-we</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>averageWordLength</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>WPT-since</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>bigraph-co</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>might</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>bigraph-we</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>uppercaseFraction</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>awps</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>since</c:v>
-                </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>apostrophesPerWord</c:v>
                 </c:pt>
-                <c:pt idx="28">
-                  <c:v>averageParagraphLength</c:v>
-                </c:pt>
                 <c:pt idx="29">
-                  <c:v>" </c:v>
+                  <c:v>WPT-quote</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>bigraph-me</c:v>
@@ -369,97 +374,97 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>6.0170000000000003</c:v>
+                  <c:v>6.2679999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.6920000000000002</c:v>
+                  <c:v>5.9649999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.67</c:v>
+                  <c:v>5.9119999999999902</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.5780000000000003</c:v>
+                  <c:v>5.8379999999999903</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.5190000000000001</c:v>
+                  <c:v>5.8259999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.4740000000000002</c:v>
+                  <c:v>5.798</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.4739999999999904</c:v>
+                  <c:v>5.0259999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.4819999999999904</c:v>
+                  <c:v>4.6950000000000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.3419999999999996</c:v>
+                  <c:v>4.6829999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.0880000000000001</c:v>
+                  <c:v>4.4669999999999996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.077</c:v>
+                  <c:v>4.4429999999999996</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.0540000000000003</c:v>
+                  <c:v>4.2889999999999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.0529999999999902</c:v>
+                  <c:v>4.0860000000000003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.9830000000000001</c:v>
+                  <c:v>4.085</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.88</c:v>
+                  <c:v>3.9849999999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.69599999999999</c:v>
+                  <c:v>3.9099999999999899</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.5</c:v>
+                  <c:v>3.8719999999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.3479999999999999</c:v>
+                  <c:v>3.4519999999999902</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.3359999999999999</c:v>
+                  <c:v>3.4140000000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.1749999999999998</c:v>
+                  <c:v>3.3119999999999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.1640000000000001</c:v>
+                  <c:v>3.0960000000000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.9790000000000001</c:v>
+                  <c:v>3.0710000000000002</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.944</c:v>
+                  <c:v>2.99399999999999</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.863</c:v>
+                  <c:v>2.88</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.8540000000000001</c:v>
+                  <c:v>2.879</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.8519999999999999</c:v>
+                  <c:v>2.879</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.75999999999999</c:v>
+                  <c:v>2.8660000000000001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.6339999999999999</c:v>
+                  <c:v>2.742</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.5169999999999999</c:v>
+                  <c:v>2.677</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.2850000000000001</c:v>
+                  <c:v>2.637</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.744</c:v>
+                  <c:v>1.992</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -475,11 +480,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="453635824"/>
-        <c:axId val="453633080"/>
+        <c:axId val="529891312"/>
+        <c:axId val="529887392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="453635824"/>
+        <c:axId val="529891312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -505,7 +510,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Features</a:t>
                 </a:r>
               </a:p>
@@ -578,7 +583,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="453633080"/>
+        <c:crossAx val="529887392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -586,7 +591,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="453633080"/>
+        <c:axId val="529887392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -626,8 +631,8 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Accuracy</a:t>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>Accuracy (%)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -693,7 +698,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="453635824"/>
+        <c:crossAx val="529891312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1315,6 +1320,170 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11668125" y="5800725"/>
+          <a:ext cx="2314575" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>minBooks</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:effectLst/>
+            </a:rPr>
+            <a:t> = 3       authorCount = 500</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1586,7 +1755,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V22" sqref="V22"/>
+      <selection activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1596,250 +1765,250 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B1">
-        <v>6.0170000000000003</v>
+        <v>6.2679999999999998</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2">
-        <v>5.6920000000000002</v>
+        <v>5.9649999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3">
-        <v>5.67</v>
+        <v>5.9119999999999902</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4">
-        <v>5.5780000000000003</v>
+        <v>5.8379999999999903</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B5">
-        <v>5.5190000000000001</v>
+        <v>5.8259999999999996</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B6">
-        <v>5.4740000000000002</v>
+        <v>5.798</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B7">
-        <v>5.4739999999999904</v>
+        <v>5.0259999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B8">
-        <v>4.4819999999999904</v>
+        <v>4.6950000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B9">
-        <v>4.3419999999999996</v>
+        <v>4.6829999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B10">
-        <v>4.0880000000000001</v>
+        <v>4.4669999999999996</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B11">
-        <v>4.077</v>
+        <v>4.4429999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B12">
-        <v>4.0540000000000003</v>
+        <v>4.2889999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B13">
-        <v>4.0529999999999902</v>
+        <v>4.0860000000000003</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B14">
-        <v>3.9830000000000001</v>
+        <v>4.085</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B15">
-        <v>3.88</v>
+        <v>3.9849999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B16">
-        <v>3.69599999999999</v>
+        <v>3.9099999999999899</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>3.5</v>
+        <v>3.8719999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B18">
-        <v>3.3479999999999999</v>
+        <v>3.4519999999999902</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B19">
-        <v>3.3359999999999999</v>
+        <v>3.4140000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B20">
-        <v>3.1749999999999998</v>
+        <v>3.3119999999999998</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B21">
-        <v>3.1640000000000001</v>
+        <v>3.0960000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B22">
-        <v>2.9790000000000001</v>
+        <v>3.0710000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B23">
-        <v>2.944</v>
+        <v>2.99399999999999</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B24">
-        <v>2.863</v>
+        <v>2.88</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="B25">
-        <v>2.8540000000000001</v>
+        <v>2.879</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B26">
-        <v>2.8519999999999999</v>
+        <v>2.879</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B27">
-        <v>2.75999999999999</v>
+        <v>2.8660000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B28">
-        <v>2.6339999999999999</v>
+        <v>2.742</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B29">
-        <v>2.5169999999999999</v>
+        <v>2.677</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B30">
-        <v>2.2850000000000001</v>
+        <v>2.637</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B31">
-        <v>1.744</v>
+        <v>1.992</v>
       </c>
     </row>
   </sheetData>

</xml_diff>